<commit_message>
Convert Automation to Excel Buffer in report
</commit_message>
<xml_diff>
--- a/Excel Export.xlsx
+++ b/Excel Export.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Customers" sheetId="1" r:id="R1c287c53dc744f7f"/>
-    <x:sheet name="Vendors" sheetId="2" r:id="Rc8ce83969b0a4225"/>
-    <x:sheet name="Items" sheetId="3" r:id="Ra44c0fe3e0e64c86"/>
+    <x:sheet name="Customers" sheetId="1" r:id="R1112c63c0d594b4d"/>
+    <x:sheet name="Vendors" sheetId="2" r:id="R106743b1d317473c"/>
+    <x:sheet name="Items" sheetId="3" r:id="Rd0302f5671a64f39"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -263,37 +263,6 @@
         <x:v>44714</x:v>
       </x:c>
     </x:row>
-    <x:row r="6">
-      <x:c r="A6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">50000</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Relecloud</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Atlanta</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Jesse Homer</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E6" s="3" t="inlineStr">
-        <x:v/>
-        <x:is>
-          <x:t xml:space="preserve">jesse.homer@contoso.com</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F6" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:pageSetup paperSize="9" orientation="landscape"/>
   <x:headerFooter>
@@ -303,7 +272,7 @@
 VLADEK
 Page &amp;P</x:evenHeader>
   </x:headerFooter>
-  <x:legacyDrawing r:id="R21c787bba86d4b3a"/>
+  <x:legacyDrawing r:id="R96e7298bb7f74111"/>
 </x:worksheet>
 </file>
 
@@ -470,36 +439,6 @@
         <x:v>44714</x:v>
       </x:c>
     </x:row>
-    <x:row r="6">
-      <x:c r="A6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">50000</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Nod Publishers</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Atlanta</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Raymond Hillard</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">NOD PUBLISHERS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="F6" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:pageSetup paperSize="9" orientation="landscape"/>
   <x:headerFooter>
@@ -509,7 +448,7 @@
 VLADEK
 Page &amp;P</x:evenHeader>
   </x:headerFooter>
-  <x:legacyDrawing r:id="R1c574cf1e66c449f"/>
+  <x:legacyDrawing r:id="Rf5906aa6ced14676"/>
 </x:worksheet>
 </file>
 
@@ -537,20 +476,25 @@
       </x:c>
       <x:c r="C1" s="1" t="inlineStr">
         <x:is>
+          <x:t xml:space="preserve">Base Unit of Measure</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D1" s="1" t="inlineStr">
+        <x:is>
           <x:t xml:space="preserve">Type</x:t>
         </x:is>
       </x:c>
-      <x:c r="D1" s="1" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Base Unit of Measure</x:t>
-        </x:is>
-      </x:c>
       <x:c r="E1" s="1" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Unit Cost</x:t>
         </x:is>
       </x:c>
       <x:c r="F1" s="1" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">Item Category Code</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G1" s="1" t="inlineStr">
         <x:is>
           <x:t xml:space="preserve">Last Date Modified</x:t>
         </x:is>
@@ -569,18 +513,23 @@
       </x:c>
       <x:c r="C2" s="2" t="inlineStr">
         <x:is>
+          <x:t xml:space="preserve">PCS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D2" s="2" t="inlineStr">
+        <x:is>
           <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D2" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
         </x:is>
       </x:c>
       <x:c r="E2" s="0" t="n">
         <x:v>780.7</x:v>
       </x:c>
-      <x:c r="F2" s="4" t="n">
+      <x:c r="F2" s="2" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">TABLE</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G2" s="4" t="n">
         <x:v>44714</x:v>
       </x:c>
     </x:row>
@@ -597,18 +546,23 @@
       </x:c>
       <x:c r="C3" s="2" t="inlineStr">
         <x:is>
+          <x:t xml:space="preserve">PCS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D3" s="2" t="inlineStr">
+        <x:is>
           <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D3" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
         </x:is>
       </x:c>
       <x:c r="E3" s="0" t="n">
         <x:v>150.3</x:v>
       </x:c>
-      <x:c r="F3" s="4" t="n">
+      <x:c r="F3" s="2" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CHAIR</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G3" s="4" t="n">
         <x:v>44714</x:v>
       </x:c>
     </x:row>
@@ -625,18 +579,23 @@
       </x:c>
       <x:c r="C4" s="2" t="inlineStr">
         <x:is>
+          <x:t xml:space="preserve">PCS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D4" s="2" t="inlineStr">
+        <x:is>
           <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D4" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
         </x:is>
       </x:c>
       <x:c r="E4" s="0" t="n">
         <x:v>338.2</x:v>
       </x:c>
-      <x:c r="F4" s="4" t="n">
+      <x:c r="F4" s="2" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">TABLE</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G4" s="4" t="n">
         <x:v>44714</x:v>
       </x:c>
     </x:row>
@@ -653,186 +612,23 @@
       </x:c>
       <x:c r="C5" s="2" t="inlineStr">
         <x:is>
+          <x:t xml:space="preserve">PCS</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="D5" s="2" t="inlineStr">
+        <x:is>
           <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D5" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
         </x:is>
       </x:c>
       <x:c r="E5" s="0" t="n">
         <x:v>148.1</x:v>
       </x:c>
-      <x:c r="F5" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6">
-      <x:c r="A6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">1920-S</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">ANTWERP Conference Table</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D6" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E6" s="0" t="n">
-        <x:v>505.4</x:v>
-      </x:c>
-      <x:c r="F6" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7">
-      <x:c r="A7" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">1925-W</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B7" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Conference Bundle 1-6</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C7" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D7" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E7" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F7" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8">
-      <x:c r="A8" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">1928-S</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B8" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">AMSTERDAM Lamp</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C8" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D8" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E8" s="0" t="n">
-        <x:v>42.8</x:v>
-      </x:c>
-      <x:c r="F8" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9">
-      <x:c r="A9" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">1929-W</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B9" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Conference Bundle 1-8</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C9" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D9" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E9" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F9" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10">
-      <x:c r="A10" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">1936-S</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B10" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">BERLIN Guest Chair, yellow</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C10" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D10" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E10" s="0" t="n">
-        <x:v>150.3</x:v>
-      </x:c>
-      <x:c r="F10" s="4" t="n">
-        <x:v>44714</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11">
-      <x:c r="A11" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">1953-W</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B11" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Guest Section 1</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C11" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">Inventory</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="D11" s="2" t="inlineStr">
-        <x:is>
-          <x:t xml:space="preserve">PCS</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="E11" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F11" s="4" t="n">
+      <x:c r="F5" s="2" t="inlineStr">
+        <x:is>
+          <x:t xml:space="preserve">CHAIR</x:t>
+        </x:is>
+      </x:c>
+      <x:c r="G5" s="4" t="n">
         <x:v>44714</x:v>
       </x:c>
     </x:row>
@@ -845,6 +641,6 @@
 VLADEK
 Page &amp;P</x:evenHeader>
   </x:headerFooter>
-  <x:legacyDrawing r:id="R2bd1b1d14c1e4805"/>
+  <x:legacyDrawing r:id="Re2a4e89f9975445d"/>
 </x:worksheet>
 </file>
</xml_diff>